<commit_message>
last few updates from toofastdan
</commit_message>
<xml_diff>
--- a/US News Data/2021 US News Primary Care Ranks.xlsx
+++ b/US News Data/2021 US News Primary Care Ranks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ToofastDan\Documents\MD_PhD Application\SDN_Physician_Scientist_Analysis\US News Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TooFastDan\Documents\MD_PhD Application\Python Analysis\US News Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D1C279-0CCD-4D43-B621-A9A2A89641DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E10DD7-D237-4BC7-8E5E-5BE585034E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1223,6 +1223,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1275,11 +1278,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1622,20 +1626,20 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67" customWidth="1"/>
-    <col min="3" max="3" width="31.109375" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1658,7 +1662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1671,17 +1675,17 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>37760</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>69186</v>
       </c>
       <c r="G2">
         <v>1123</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1694,17 +1698,17 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>36342</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>48587</v>
       </c>
       <c r="G3">
         <v>664</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1717,17 +1721,17 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>32746</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>60140</v>
       </c>
       <c r="G4">
         <v>782</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1740,17 +1744,17 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>44356</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>68184</v>
       </c>
       <c r="G5">
         <v>617</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1763,17 +1767,17 @@
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>40191</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>57678</v>
       </c>
       <c r="G6">
         <v>1051</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1786,17 +1790,17 @@
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>41156</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>67110</v>
       </c>
       <c r="G7">
         <v>719</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1809,17 +1813,17 @@
       <c r="D8">
         <v>6</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>35362</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>57288</v>
       </c>
       <c r="G8">
         <v>513</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1832,14 +1836,15 @@
       <c r="D9">
         <v>8</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>64984</v>
       </c>
+      <c r="F9" s="2"/>
       <c r="G9">
         <v>700</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1852,17 +1857,17 @@
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>37891</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>67086</v>
       </c>
       <c r="G10">
         <v>854</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1875,17 +1880,17 @@
       <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>36570</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>62889</v>
       </c>
       <c r="G11">
         <v>670</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1898,17 +1903,17 @@
       <c r="D12">
         <v>11</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>39032</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>51277</v>
       </c>
       <c r="G12">
         <v>477</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1921,17 +1926,17 @@
       <c r="D13">
         <v>12</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>37620</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>49865</v>
       </c>
       <c r="G13">
         <v>792</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1944,17 +1949,17 @@
       <c r="D14">
         <v>12</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>38143</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>54319</v>
       </c>
       <c r="G14">
         <v>704</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1967,14 +1972,15 @@
       <c r="D15">
         <v>14</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>61500</v>
       </c>
+      <c r="F15" s="2"/>
       <c r="G15">
         <v>434</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1987,17 +1993,17 @@
       <c r="D16">
         <v>15</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>41790</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>60240</v>
       </c>
       <c r="G16">
         <v>707</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2010,17 +2016,17 @@
       <c r="D17">
         <v>16</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>37810</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>66905</v>
       </c>
       <c r="G17">
         <v>622</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2033,14 +2039,15 @@
       <c r="D18">
         <v>17</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>19425</v>
       </c>
+      <c r="F18" s="2"/>
       <c r="G18">
         <v>753</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2053,14 +2060,15 @@
       <c r="D19">
         <v>17</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>73348</v>
       </c>
+      <c r="F19" s="2"/>
       <c r="G19">
         <v>818</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2073,14 +2081,15 @@
       <c r="D20">
         <v>19</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>64974</v>
       </c>
+      <c r="F20" s="2"/>
       <c r="G20">
         <v>590</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2093,17 +2102,17 @@
       <c r="D21">
         <v>19</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>43828</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>53952</v>
       </c>
       <c r="G21">
         <v>621</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2116,17 +2125,17 @@
       <c r="D22">
         <v>21</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>29702</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>62714</v>
       </c>
       <c r="G22">
         <v>799</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -2139,14 +2148,15 @@
       <c r="D23">
         <v>22</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>62193</v>
       </c>
+      <c r="F23" s="2"/>
       <c r="G23">
         <v>484</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2159,17 +2169,17 @@
       <c r="D24">
         <v>22</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>36382</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>57157</v>
       </c>
       <c r="G24">
         <v>605</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2182,14 +2192,15 @@
       <c r="D25">
         <v>24</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>67532</v>
       </c>
+      <c r="F25" s="2"/>
       <c r="G25">
         <v>395</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2202,17 +2213,17 @@
       <c r="D26">
         <v>24</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>36672</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>73128</v>
       </c>
       <c r="G26">
         <v>305</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -2225,14 +2236,15 @@
       <c r="D27">
         <v>24</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>59910</v>
       </c>
+      <c r="F27" s="2"/>
       <c r="G27">
         <v>616</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -2245,17 +2257,17 @@
       <c r="D28">
         <v>24</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>37070</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>64170</v>
       </c>
       <c r="G28">
         <v>487</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -2268,14 +2280,15 @@
       <c r="D29">
         <v>28</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>20252</v>
       </c>
+      <c r="F29" s="2"/>
       <c r="G29">
         <v>346</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -2288,17 +2301,17 @@
       <c r="D30">
         <v>28</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>29680</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>54600</v>
       </c>
       <c r="G30">
         <v>821</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -2311,17 +2324,17 @@
       <c r="D31">
         <v>28</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>36156</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>48401</v>
       </c>
       <c r="G31">
         <v>553</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2334,17 +2347,17 @@
       <c r="D32">
         <v>28</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>15328</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>44023</v>
       </c>
       <c r="G32">
         <v>418</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -2357,17 +2370,17 @@
       <c r="D33">
         <v>32</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>20453</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>33553</v>
       </c>
       <c r="G33">
         <v>892</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -2380,17 +2393,17 @@
       <c r="D34">
         <v>32</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>40943</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>77513</v>
       </c>
       <c r="G34">
         <v>481</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -2403,14 +2416,15 @@
       <c r="D35">
         <v>34</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <v>56550</v>
       </c>
+      <c r="F35" s="2"/>
       <c r="G35">
         <v>364</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2423,17 +2437,17 @@
       <c r="D36">
         <v>34</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>57684</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>59930</v>
       </c>
       <c r="G36">
         <v>599</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2446,14 +2460,15 @@
       <c r="D37">
         <v>36</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
         <v>51000</v>
       </c>
+      <c r="F37" s="2"/>
       <c r="G37">
         <v>565</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -2466,17 +2481,17 @@
       <c r="D38">
         <v>36</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>36036</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>61419</v>
       </c>
       <c r="G38">
         <v>1441</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -2489,14 +2504,15 @@
       <c r="D39">
         <v>36</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
         <v>60870</v>
       </c>
+      <c r="F39" s="2"/>
       <c r="G39">
         <v>409</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2509,14 +2525,15 @@
       <c r="D40">
         <v>39</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>64262</v>
       </c>
+      <c r="F40" s="2"/>
       <c r="G40">
         <v>653</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -2529,17 +2546,17 @@
       <c r="D41">
         <v>39</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>33010</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>65180</v>
       </c>
       <c r="G41">
         <v>704</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -2552,14 +2569,15 @@
       <c r="D42">
         <v>41</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>58900</v>
       </c>
+      <c r="F42" s="2"/>
       <c r="G42">
         <v>420</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2572,14 +2590,15 @@
       <c r="D43">
         <v>41</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="2">
         <v>0</v>
       </c>
+      <c r="F43" s="2"/>
       <c r="G43">
         <v>417</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -2592,17 +2611,17 @@
       <c r="D44">
         <v>41</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="2">
         <v>35220</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="2">
         <v>47465</v>
       </c>
       <c r="G44">
         <v>420</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2615,14 +2634,15 @@
       <c r="D45">
         <v>44</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="2">
         <v>64884</v>
       </c>
+      <c r="F45" s="2"/>
       <c r="G45">
         <v>663</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2635,17 +2655,17 @@
       <c r="D46">
         <v>44</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="2">
         <v>40287</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="2">
         <v>74367</v>
       </c>
       <c r="G46">
         <v>449</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -2658,17 +2678,17 @@
       <c r="D47">
         <v>46</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="2">
         <v>33105</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="2">
         <v>56382</v>
       </c>
       <c r="G47">
         <v>594</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2681,14 +2701,15 @@
       <c r="D48">
         <v>46</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="2">
         <v>57260</v>
       </c>
+      <c r="F48" s="2"/>
       <c r="G48">
         <v>727</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -2701,17 +2722,17 @@
       <c r="D49">
         <v>46</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="2">
         <v>33674</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="2">
         <v>34289</v>
       </c>
       <c r="G49">
         <v>477</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -2724,14 +2745,15 @@
       <c r="D50">
         <v>46</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="2">
         <v>66150</v>
       </c>
+      <c r="F50" s="2"/>
       <c r="G50">
         <v>749</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -2744,17 +2766,17 @@
       <c r="D51">
         <v>46</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="2">
         <v>16921</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="2">
         <v>33587</v>
       </c>
       <c r="G51">
         <v>860</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -2767,14 +2789,15 @@
       <c r="D52">
         <v>51</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="2">
         <v>61110</v>
       </c>
+      <c r="F52" s="2"/>
       <c r="G52">
         <v>439</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -2787,14 +2810,15 @@
       <c r="D53">
         <v>51</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="2">
         <v>61170</v>
       </c>
+      <c r="F53" s="2"/>
       <c r="G53">
         <v>502</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -2807,14 +2831,15 @@
       <c r="D54">
         <v>51</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="2">
         <v>65052</v>
       </c>
+      <c r="F54" s="2"/>
       <c r="G54">
         <v>809</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -2827,17 +2852,17 @@
       <c r="D55">
         <v>51</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="2">
         <v>32744</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="2">
         <v>45000</v>
       </c>
       <c r="G55">
         <v>570</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -2850,17 +2875,17 @@
       <c r="D56">
         <v>51</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="2">
         <v>26770</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="2">
         <v>61098</v>
       </c>
       <c r="G56">
         <v>663</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -2873,17 +2898,17 @@
       <c r="D57">
         <v>51</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="2">
         <v>33751</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="2">
         <v>56577</v>
       </c>
       <c r="G57">
         <v>765</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -2896,17 +2921,17 @@
       <c r="D58">
         <v>57</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="2">
         <v>13078</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="2">
         <v>28766</v>
       </c>
       <c r="G58">
         <v>945</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -2919,17 +2944,17 @@
       <c r="D59">
         <v>58</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="2">
         <v>33580</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="2">
         <v>54180</v>
       </c>
       <c r="G59">
         <v>492</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -2942,14 +2967,15 @@
       <c r="D60">
         <v>59</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="2">
         <v>56500</v>
       </c>
+      <c r="F60" s="2"/>
       <c r="G60">
         <v>477</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -2962,14 +2988,15 @@
       <c r="D61">
         <v>59</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="2">
         <v>58557</v>
       </c>
+      <c r="F61" s="2"/>
       <c r="G61">
         <v>1088</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -2982,17 +3009,17 @@
       <c r="D62">
         <v>59</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="2">
         <v>32980</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="2">
         <v>51244</v>
       </c>
       <c r="G62">
         <v>721</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -3005,14 +3032,15 @@
       <c r="D63">
         <v>59</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="2">
         <v>64231</v>
       </c>
+      <c r="F63" s="2"/>
       <c r="G63">
         <v>448</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -3025,14 +3053,15 @@
       <c r="D64">
         <v>59</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="2">
         <v>64864</v>
       </c>
+      <c r="F64" s="2"/>
       <c r="G64">
         <v>394</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -3045,17 +3074,17 @@
       <c r="D65">
         <v>64</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="2">
         <v>32834</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="2">
         <v>42684</v>
       </c>
       <c r="G65">
         <v>291</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -3068,17 +3097,17 @@
       <c r="D66">
         <v>64</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="2">
         <v>31890</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="2">
         <v>63780</v>
       </c>
       <c r="G66">
         <v>489</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -3091,14 +3120,15 @@
       <c r="D67">
         <v>66</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="2">
         <v>64868</v>
       </c>
+      <c r="F67" s="2"/>
       <c r="G67">
         <v>585</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -3111,17 +3141,17 @@
       <c r="D68">
         <v>67</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="2">
         <v>45360</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="2">
         <v>78537</v>
       </c>
       <c r="G68">
         <v>1275</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -3134,17 +3164,17 @@
       <c r="D69">
         <v>67</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="2">
         <v>30672</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="2">
         <v>62181</v>
       </c>
       <c r="G69">
         <v>456</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -3157,14 +3187,15 @@
       <c r="D70">
         <v>69</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="2">
         <v>55052</v>
       </c>
+      <c r="F70" s="2"/>
       <c r="G70">
         <v>777</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -3177,14 +3208,15 @@
       <c r="D71">
         <v>69</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="2">
         <v>56975</v>
       </c>
+      <c r="F71" s="2"/>
       <c r="G71">
         <v>584</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -3197,14 +3229,15 @@
       <c r="D72">
         <v>69</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="2">
         <v>57010</v>
       </c>
+      <c r="F72" s="2"/>
       <c r="G72">
         <v>572</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -3217,17 +3250,17 @@
       <c r="D73">
         <v>69</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="2">
         <v>16320</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="2">
         <v>29820</v>
       </c>
       <c r="G73">
         <v>737</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -3240,17 +3273,17 @@
       <c r="D74">
         <v>69</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="2">
         <v>29175</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="2">
         <v>49355</v>
       </c>
       <c r="G74">
         <v>730</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -3263,14 +3296,15 @@
       <c r="D75">
         <v>74</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="2">
         <v>67440</v>
       </c>
+      <c r="F75" s="2"/>
       <c r="G75">
         <v>917</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -3283,17 +3317,17 @@
       <c r="D76">
         <v>74</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="2">
         <v>41778</v>
       </c>
-      <c r="F76">
+      <c r="F76" s="2">
         <v>63530</v>
       </c>
       <c r="G76">
         <v>654</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -3306,14 +3340,15 @@
       <c r="D77">
         <v>76</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="2">
         <v>52200</v>
       </c>
+      <c r="F77" s="2"/>
       <c r="G77">
         <v>402</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -3326,17 +3361,17 @@
       <c r="D78">
         <v>76</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="2">
         <v>42888</v>
       </c>
-      <c r="F78">
+      <c r="F78" s="2">
         <v>87150</v>
       </c>
       <c r="G78">
         <v>403</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -3349,14 +3384,15 @@
       <c r="D79">
         <v>78</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="2">
         <v>62060</v>
       </c>
+      <c r="F79" s="2"/>
       <c r="G79">
         <v>721</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -3369,17 +3405,17 @@
       <c r="D80">
         <v>79</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="2">
         <v>22408</v>
       </c>
-      <c r="F80">
+      <c r="F80" s="2">
         <v>55314</v>
       </c>
       <c r="G80">
         <v>490</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -3392,14 +3428,15 @@
       <c r="D81">
         <v>80</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="2">
         <v>36000</v>
       </c>
+      <c r="F81" s="2"/>
       <c r="G81">
         <v>2390</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -3412,8 +3449,10 @@
       <c r="D82">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -3426,14 +3465,15 @@
       <c r="D83">
         <v>80</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="2">
         <v>61200</v>
       </c>
+      <c r="F83" s="2"/>
       <c r="G83">
         <v>580</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -3446,17 +3486,17 @@
       <c r="D84">
         <v>80</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="2">
         <v>37728</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="2">
         <v>56606</v>
       </c>
       <c r="G84">
         <v>481</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>90</v>
       </c>
@@ -3469,14 +3509,15 @@
       <c r="D85">
         <v>84</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="2">
         <v>46610</v>
       </c>
+      <c r="F85" s="2"/>
       <c r="G85">
         <v>476</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>91</v>
       </c>
@@ -3489,17 +3530,17 @@
       <c r="D86">
         <v>84</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="2">
         <v>53406</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="2">
         <v>56628</v>
       </c>
       <c r="G86">
         <v>875</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>92</v>
       </c>
@@ -3512,17 +3553,17 @@
       <c r="D87">
         <v>84</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="2">
         <v>16220</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="2">
         <v>29320</v>
       </c>
       <c r="G87">
         <v>582</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -3535,17 +3576,17 @@
       <c r="D88">
         <v>84</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="2">
         <v>29386</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="2">
         <v>57704</v>
       </c>
       <c r="G88">
         <v>286</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -3558,17 +3599,17 @@
       <c r="D89">
         <v>84</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="2">
         <v>17872</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="2">
         <v>26125</v>
       </c>
       <c r="G89">
         <v>979</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -3581,14 +3622,15 @@
       <c r="D90">
         <v>89</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="2">
         <v>55072</v>
       </c>
+      <c r="F90" s="2"/>
       <c r="G90">
         <v>809</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -3601,17 +3643,17 @@
       <c r="D91">
         <v>89</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="2">
         <v>35571</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="2">
         <v>62949</v>
       </c>
       <c r="G91">
         <v>1188</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>97</v>
       </c>
@@ -3624,17 +3666,17 @@
       <c r="D92">
         <v>91</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="2">
         <v>28296</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="2">
         <v>57850</v>
       </c>
       <c r="G92">
         <v>942</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>98</v>
       </c>
@@ -3647,17 +3689,17 @@
       <c r="D93">
         <v>91</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="2">
         <v>43670</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="2">
         <v>65160</v>
       </c>
       <c r="G93">
         <v>727</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>99</v>
       </c>
@@ -3670,17 +3712,17 @@
       <c r="D94" t="s">
         <v>397</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="2">
         <v>40479</v>
       </c>
-      <c r="F94">
+      <c r="F94" s="2">
         <v>64240</v>
       </c>
       <c r="G94">
         <v>432</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>100</v>
       </c>
@@ -3693,14 +3735,15 @@
       <c r="D95" t="s">
         <v>397</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="2">
         <v>58978</v>
       </c>
+      <c r="F95" s="2"/>
       <c r="G95">
         <v>1062</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>101</v>
       </c>
@@ -3713,14 +3756,15 @@
       <c r="D96" t="s">
         <v>397</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="2">
         <v>46900</v>
       </c>
+      <c r="F96" s="2"/>
       <c r="G96">
         <v>2122</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>102</v>
       </c>
@@ -3733,17 +3777,17 @@
       <c r="D97" t="s">
         <v>397</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="2">
         <v>28111</v>
       </c>
-      <c r="F97">
+      <c r="F97" s="2">
         <v>62532</v>
       </c>
       <c r="G97">
         <v>253</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -3756,17 +3800,17 @@
       <c r="D98" t="s">
         <v>397</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="2">
         <v>32737</v>
       </c>
-      <c r="F98">
+      <c r="F98" s="2">
         <v>62737</v>
       </c>
       <c r="G98">
         <v>484</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>104</v>
       </c>
@@ -3779,14 +3823,15 @@
       <c r="D99" t="s">
         <v>397</v>
       </c>
-      <c r="E99">
+      <c r="E99" s="2">
         <v>52650</v>
       </c>
+      <c r="F99" s="2"/>
       <c r="G99">
         <v>1191</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>105</v>
       </c>
@@ -3799,17 +3844,17 @@
       <c r="D100" t="s">
         <v>397</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="2">
         <v>28592</v>
       </c>
-      <c r="F100">
+      <c r="F100" s="2">
         <v>60414</v>
       </c>
       <c r="G100">
         <v>551</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>106</v>
       </c>
@@ -3822,17 +3867,17 @@
       <c r="D101" t="s">
         <v>397</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="2">
         <v>24004</v>
       </c>
-      <c r="F101">
+      <c r="F101" s="2">
         <v>56788</v>
       </c>
       <c r="G101">
         <v>326</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>24</v>
       </c>
@@ -3845,14 +3890,15 @@
       <c r="D102" t="s">
         <v>397</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="2">
         <v>71146</v>
       </c>
+      <c r="F102" s="2"/>
       <c r="G102">
         <v>1021</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>107</v>
       </c>
@@ -3865,14 +3911,15 @@
       <c r="D103" t="s">
         <v>397</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="2">
         <v>55670</v>
       </c>
+      <c r="F103" s="2"/>
       <c r="G103">
         <v>857</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>108</v>
       </c>
@@ -3885,14 +3932,15 @@
       <c r="D104" t="s">
         <v>397</v>
       </c>
-      <c r="E104">
+      <c r="E104" s="2">
         <v>55671</v>
       </c>
+      <c r="F104" s="2"/>
       <c r="G104">
         <v>1302</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>109</v>
       </c>
@@ -3905,17 +3953,17 @@
       <c r="D105" t="s">
         <v>397</v>
       </c>
-      <c r="E105">
+      <c r="E105" s="2">
         <v>37068</v>
       </c>
-      <c r="F105">
+      <c r="F105" s="2">
         <v>52864</v>
       </c>
       <c r="G105">
         <v>993</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>110</v>
       </c>
@@ -3928,17 +3976,17 @@
       <c r="D106" t="s">
         <v>397</v>
       </c>
-      <c r="E106">
+      <c r="E106" s="2">
         <v>25797</v>
       </c>
-      <c r="F106">
+      <c r="F106" s="2">
         <v>53299</v>
       </c>
       <c r="G106">
         <v>524</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>111</v>
       </c>
@@ -3951,14 +3999,15 @@
       <c r="D107" t="s">
         <v>397</v>
       </c>
-      <c r="E107">
+      <c r="E107" s="2">
         <v>59830</v>
       </c>
+      <c r="F107" s="2"/>
       <c r="G107">
         <v>394</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>112</v>
       </c>
@@ -3971,17 +4020,17 @@
       <c r="D108" t="s">
         <v>397</v>
       </c>
-      <c r="E108">
+      <c r="E108" s="2">
         <v>41339</v>
       </c>
-      <c r="F108">
+      <c r="F108" s="2">
         <v>66324</v>
       </c>
       <c r="G108">
         <v>817</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>113</v>
       </c>
@@ -3994,17 +4043,17 @@
       <c r="D109" t="s">
         <v>397</v>
       </c>
-      <c r="E109">
+      <c r="E109" s="2">
         <v>41281</v>
       </c>
-      <c r="F109">
+      <c r="F109" s="2">
         <v>63697</v>
       </c>
       <c r="G109">
         <v>760</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>114</v>
       </c>
@@ -4017,17 +4066,17 @@
       <c r="D110" t="s">
         <v>397</v>
       </c>
-      <c r="E110">
+      <c r="E110" s="2">
         <v>43345</v>
       </c>
-      <c r="F110">
+      <c r="F110" s="2">
         <v>66881</v>
       </c>
       <c r="G110">
         <v>743</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>115</v>
       </c>
@@ -4040,17 +4089,17 @@
       <c r="D111" t="s">
         <v>397</v>
       </c>
-      <c r="E111">
+      <c r="E111" s="2">
         <v>43670</v>
       </c>
-      <c r="F111">
+      <c r="F111" s="2">
         <v>65160</v>
       </c>
       <c r="G111">
         <v>567</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>116</v>
       </c>
@@ -4063,17 +4112,17 @@
       <c r="D112" t="s">
         <v>397</v>
       </c>
-      <c r="E112">
+      <c r="E112" s="2">
         <v>43670</v>
       </c>
-      <c r="F112">
+      <c r="F112" s="2">
         <v>65160</v>
       </c>
       <c r="G112">
         <v>675</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>117</v>
       </c>
@@ -4086,14 +4135,15 @@
       <c r="D113" t="s">
         <v>397</v>
       </c>
-      <c r="E113">
+      <c r="E113" s="2">
         <v>58000</v>
       </c>
+      <c r="F113" s="2"/>
       <c r="G113">
         <v>543</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>118</v>
       </c>
@@ -4106,17 +4156,17 @@
       <c r="D114" t="s">
         <v>397</v>
       </c>
-      <c r="E114">
+      <c r="E114" s="2">
         <v>36630</v>
       </c>
-      <c r="F114">
+      <c r="F114" s="2">
         <v>48875</v>
       </c>
       <c r="G114">
         <v>299</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>119</v>
       </c>
@@ -4129,17 +4179,17 @@
       <c r="D115" t="s">
         <v>397</v>
       </c>
-      <c r="E115">
+      <c r="E115" s="2">
         <v>25491</v>
       </c>
-      <c r="F115">
+      <c r="F115" s="2">
         <v>52365</v>
       </c>
       <c r="G115">
         <v>490</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>120</v>
       </c>
@@ -4152,17 +4202,17 @@
       <c r="D116" t="s">
         <v>397</v>
       </c>
-      <c r="E116">
+      <c r="E116" s="2">
         <v>38938</v>
       </c>
-      <c r="F116">
+      <c r="F116" s="2">
         <v>72330</v>
       </c>
       <c r="G116">
         <v>718</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>121</v>
       </c>
@@ -4175,14 +4225,15 @@
       <c r="D117" t="s">
         <v>397</v>
       </c>
-      <c r="E117">
+      <c r="E117" s="2">
         <v>47476</v>
       </c>
+      <c r="F117" s="2"/>
       <c r="G117">
         <v>841</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>122</v>
       </c>
@@ -4195,14 +4246,15 @@
       <c r="D118" t="s">
         <v>397</v>
       </c>
-      <c r="E118">
+      <c r="E118" s="2">
         <v>58430</v>
       </c>
+      <c r="F118" s="2"/>
       <c r="G118">
         <v>702</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>123</v>
       </c>
@@ -4215,14 +4267,15 @@
       <c r="D119" t="s">
         <v>397</v>
       </c>
-      <c r="E119">
+      <c r="E119" s="2">
         <v>48850</v>
       </c>
+      <c r="F119" s="2"/>
       <c r="G119">
         <v>552</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>124</v>
       </c>
@@ -4235,17 +4288,17 @@
       <c r="D120" t="s">
         <v>397</v>
       </c>
-      <c r="E120">
+      <c r="E120" s="2">
         <v>32908</v>
       </c>
-      <c r="F120">
+      <c r="F120" s="2">
         <v>65285</v>
       </c>
       <c r="G120">
         <v>718</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>125</v>
       </c>
@@ -4258,17 +4311,17 @@
       <c r="D121" t="s">
         <v>397</v>
       </c>
-      <c r="E121">
+      <c r="E121" s="2">
         <v>53113</v>
       </c>
-      <c r="F121">
+      <c r="F121" s="2">
         <v>53113</v>
       </c>
       <c r="G121">
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>126</v>
       </c>
@@ -4281,14 +4334,15 @@
       <c r="D122" t="s">
         <v>397</v>
       </c>
-      <c r="E122">
+      <c r="E122" s="2">
         <v>59560</v>
       </c>
+      <c r="F122" s="2"/>
       <c r="G122">
         <v>1339</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>127</v>
       </c>
@@ -4301,17 +4355,17 @@
       <c r="D123" t="s">
         <v>397</v>
       </c>
-      <c r="E123">
+      <c r="E123" s="2">
         <v>21472</v>
       </c>
-      <c r="F123">
+      <c r="F123" s="2">
         <v>52710</v>
       </c>
       <c r="G123">
         <v>800</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>128</v>
       </c>
@@ -4324,14 +4378,15 @@
       <c r="D124" t="s">
         <v>397</v>
       </c>
-      <c r="E124">
+      <c r="E124" s="2">
         <v>44000</v>
       </c>
+      <c r="F124" s="2"/>
       <c r="G124">
         <v>455</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>129</v>
       </c>
@@ -4344,8 +4399,10 @@
       <c r="D125" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>130</v>
       </c>
@@ -4358,8 +4415,10 @@
       <c r="D126" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>131</v>
       </c>
@@ -4372,8 +4431,10 @@
       <c r="D127" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>132</v>
       </c>
@@ -4386,8 +4447,10 @@
       <c r="D128" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>133</v>
       </c>
@@ -4400,8 +4463,10 @@
       <c r="D129" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>134</v>
       </c>
@@ -4414,8 +4479,10 @@
       <c r="D130" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>135</v>
       </c>
@@ -4428,8 +4495,10 @@
       <c r="D131" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E131" s="2"/>
+      <c r="F131" s="2"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>136</v>
       </c>
@@ -4442,8 +4511,10 @@
       <c r="D132" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E132" s="2"/>
+      <c r="F132" s="2"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>137</v>
       </c>
@@ -4456,14 +4527,15 @@
       <c r="D133" t="s">
         <v>398</v>
       </c>
-      <c r="E133">
+      <c r="E133" s="2">
         <v>58500</v>
       </c>
+      <c r="F133" s="2"/>
       <c r="G133">
         <v>292</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>138</v>
       </c>
@@ -4476,8 +4548,10 @@
       <c r="D134" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>139</v>
       </c>
@@ -4490,8 +4564,10 @@
       <c r="D135" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>140</v>
       </c>
@@ -4504,8 +4580,10 @@
       <c r="D136" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>141</v>
       </c>
@@ -4518,8 +4596,10 @@
       <c r="D137" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>142</v>
       </c>
@@ -4532,8 +4612,10 @@
       <c r="D138" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>143</v>
       </c>
@@ -4546,8 +4628,10 @@
       <c r="D139" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>144</v>
       </c>
@@ -4560,8 +4644,10 @@
       <c r="D140" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>145</v>
       </c>
@@ -4574,14 +4660,15 @@
       <c r="D141" t="s">
         <v>398</v>
       </c>
-      <c r="E141">
+      <c r="E141" s="2">
         <v>63284</v>
       </c>
+      <c r="F141" s="2"/>
       <c r="G141">
         <v>272</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>146</v>
       </c>
@@ -4594,8 +4681,10 @@
       <c r="D142" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>147</v>
       </c>
@@ -4608,14 +4697,15 @@
       <c r="D143" t="s">
         <v>398</v>
       </c>
-      <c r="E143">
+      <c r="E143" s="2">
         <v>0</v>
       </c>
+      <c r="F143" s="2"/>
       <c r="G143">
         <v>50</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>148</v>
       </c>
@@ -4628,8 +4718,10 @@
       <c r="D144" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>149</v>
       </c>
@@ -4642,8 +4734,10 @@
       <c r="D145" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>150</v>
       </c>
@@ -4656,8 +4750,10 @@
       <c r="D146" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>151</v>
       </c>
@@ -4670,8 +4766,10 @@
       <c r="D147" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>152</v>
       </c>
@@ -4684,8 +4782,10 @@
       <c r="D148" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E148" s="2"/>
+      <c r="F148" s="2"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>153</v>
       </c>
@@ -4698,8 +4798,10 @@
       <c r="D149" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>154</v>
       </c>
@@ -4712,8 +4814,10 @@
       <c r="D150" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E150" s="2"/>
+      <c r="F150" s="2"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>155</v>
       </c>
@@ -4726,8 +4830,10 @@
       <c r="D151" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E151" s="2"/>
+      <c r="F151" s="2"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>156</v>
       </c>
@@ -4740,8 +4846,10 @@
       <c r="D152" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E152" s="2"/>
+      <c r="F152" s="2"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>157</v>
       </c>
@@ -4754,8 +4862,10 @@
       <c r="D153" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>158</v>
       </c>
@@ -4768,8 +4878,10 @@
       <c r="D154" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>159</v>
       </c>
@@ -4782,8 +4894,10 @@
       <c r="D155" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>160</v>
       </c>
@@ -4796,8 +4910,10 @@
       <c r="D156" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E156" s="2"/>
+      <c r="F156" s="2"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>161</v>
       </c>
@@ -4810,8 +4926,10 @@
       <c r="D157" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E157" s="2"/>
+      <c r="F157" s="2"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>162</v>
       </c>
@@ -4824,14 +4942,15 @@
       <c r="D158" t="s">
         <v>398</v>
       </c>
-      <c r="E158">
+      <c r="E158" s="2">
         <v>0</v>
       </c>
+      <c r="F158" s="2"/>
       <c r="G158">
         <v>47</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>163</v>
       </c>
@@ -4844,8 +4963,10 @@
       <c r="D159" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E159" s="2"/>
+      <c r="F159" s="2"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>164</v>
       </c>
@@ -4858,14 +4979,15 @@
       <c r="D160" t="s">
         <v>398</v>
       </c>
-      <c r="E160">
+      <c r="E160" s="2">
         <v>55671</v>
       </c>
+      <c r="F160" s="2"/>
       <c r="G160">
         <v>154</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>165</v>
       </c>
@@ -4878,8 +5000,10 @@
       <c r="D161" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E161" s="2"/>
+      <c r="F161" s="2"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>166</v>
       </c>
@@ -4892,8 +5016,10 @@
       <c r="D162" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E162" s="2"/>
+      <c r="F162" s="2"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>167</v>
       </c>
@@ -4906,8 +5032,10 @@
       <c r="D163" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E163" s="2"/>
+      <c r="F163" s="2"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>168</v>
       </c>
@@ -4920,8 +5048,10 @@
       <c r="D164" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E164" s="2"/>
+      <c r="F164" s="2"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>169</v>
       </c>
@@ -4934,8 +5064,10 @@
       <c r="D165" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E165" s="2"/>
+      <c r="F165" s="2"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>170</v>
       </c>
@@ -4948,8 +5080,10 @@
       <c r="D166" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>171</v>
       </c>
@@ -4962,8 +5096,10 @@
       <c r="D167" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E167" s="2"/>
+      <c r="F167" s="2"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>172</v>
       </c>
@@ -4976,8 +5112,10 @@
       <c r="D168" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E168" s="2"/>
+      <c r="F168" s="2"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>173</v>
       </c>
@@ -4990,8 +5128,10 @@
       <c r="D169" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E169" s="2"/>
+      <c r="F169" s="2"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>174</v>
       </c>
@@ -5004,8 +5144,10 @@
       <c r="D170" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E170" s="2"/>
+      <c r="F170" s="2"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>175</v>
       </c>
@@ -5018,8 +5160,10 @@
       <c r="D171" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E171" s="2"/>
+      <c r="F171" s="2"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>176</v>
       </c>
@@ -5032,14 +5176,15 @@
       <c r="D172" t="s">
         <v>398</v>
       </c>
-      <c r="E172">
+      <c r="E172" s="2">
         <v>60318</v>
       </c>
+      <c r="F172" s="2"/>
       <c r="G172">
         <v>119</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>177</v>
       </c>
@@ -5052,8 +5197,10 @@
       <c r="D173" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E173" s="2"/>
+      <c r="F173" s="2"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>178</v>
       </c>
@@ -5066,8 +5213,10 @@
       <c r="D174" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E174" s="2"/>
+      <c r="F174" s="2"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>179</v>
       </c>
@@ -5080,8 +5229,10 @@
       <c r="D175" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E175" s="2"/>
+      <c r="F175" s="2"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>180</v>
       </c>
@@ -5094,8 +5245,10 @@
       <c r="D176" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E176" s="2"/>
+      <c r="F176" s="2"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>181</v>
       </c>
@@ -5108,8 +5261,10 @@
       <c r="D177" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E177" s="2"/>
+      <c r="F177" s="2"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>182</v>
       </c>
@@ -5122,8 +5277,10 @@
       <c r="D178" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E178" s="2"/>
+      <c r="F178" s="2"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>183</v>
       </c>
@@ -5136,8 +5293,10 @@
       <c r="D179" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E179" s="2"/>
+      <c r="F179" s="2"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>184</v>
       </c>
@@ -5150,8 +5309,10 @@
       <c r="D180" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E180" s="2"/>
+      <c r="F180" s="2"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>185</v>
       </c>
@@ -5164,8 +5325,10 @@
       <c r="D181" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E181" s="2"/>
+      <c r="F181" s="2"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>186</v>
       </c>
@@ -5178,8 +5341,10 @@
       <c r="D182" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E182" s="2"/>
+      <c r="F182" s="2"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>187</v>
       </c>
@@ -5192,8 +5357,10 @@
       <c r="D183" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E183" s="2"/>
+      <c r="F183" s="2"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>188</v>
       </c>
@@ -5206,8 +5373,10 @@
       <c r="D184" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E184" s="2"/>
+      <c r="F184" s="2"/>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>189</v>
       </c>
@@ -5220,8 +5389,10 @@
       <c r="D185" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E185" s="2"/>
+      <c r="F185" s="2"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>190</v>
       </c>
@@ -5234,8 +5405,10 @@
       <c r="D186" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E186" s="2"/>
+      <c r="F186" s="2"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>191</v>
       </c>
@@ -5248,8 +5421,10 @@
       <c r="D187" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E187" s="2"/>
+      <c r="F187" s="2"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>192</v>
       </c>
@@ -5262,8 +5437,10 @@
       <c r="D188" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E188" s="2"/>
+      <c r="F188" s="2"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>193</v>
       </c>
@@ -5276,8 +5453,10 @@
       <c r="D189" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E189" s="2"/>
+      <c r="F189" s="2"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>194</v>
       </c>
@@ -5290,8 +5469,10 @@
       <c r="D190" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E190" s="2"/>
+      <c r="F190" s="2"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>195</v>
       </c>
@@ -5304,8 +5485,11 @@
       <c r="D191" t="s">
         <v>398</v>
       </c>
+      <c r="E191" s="2"/>
+      <c r="F191" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>